<commit_message>
Update malg with animation
</commit_message>
<xml_diff>
--- a/tables/gaps.xlsx
+++ b/tables/gaps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthipsey/AED Dropbox/Matt Hipsey/GitHub/cdm-science/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8CFADB84-C7B1-4E49-B253-00E3881EFBA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9B1C24-5D0B-AB4D-A84D-5519F12CAC7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11580" yWindow="5400" windowWidth="28040" windowHeight="17440" xr2:uid="{38855B1E-37A1-964D-85B5-B8485EEFAE79}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
   <si>
     <t>Data</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -185,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -195,6 +198,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,7 +518,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -688,6 +694,9 @@
       <c r="D10" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="E10" s="5" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>